<commit_message>
[LPF-987]: Enable AT's (#63)
</commit_message>
<xml_diff>
--- a/src/test/resources/expected_results/CCMS and CIS Bank Account Report w Category Code (MNTH).xlsx
+++ b/src/test/resources/expected_results/CCMS and CIS Bank Account Report w Category Code (MNTH).xlsx
@@ -3,23 +3,25 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView activeTab="1"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
+    <sheet name="MAIN" r:id="rId3" sheetId="1"/>
     <sheet name="Provider Contigency" r:id="rId4" sheetId="2"/>
-    <sheet name="MAIN" r:id="rId3" sheetId="1"/>
     <sheet name="Summary" r:id="rId5" sheetId="3"/>
-    <sheet name="Transparency Rec" r:id="rId7" sheetId="4"/>
+    <sheet name="Transparency Rec" r:id="rId9" sheetId="5"/>
+    <sheet name="By Source and Expenditure type" r:id="rId7" sheetId="4"/>
   </sheets>
   <pivotCaches>
     <pivotCache cacheId="2" r:id="rId6"/>
     <pivotCache cacheId="3" r:id="rId8"/>
+    <pivotCache cacheId="4" r:id="rId10"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>CCMS and CIS Bank Account Report (YTD)</t>
   </si>
@@ -57,6 +59,18 @@
     <t>Grand Total</t>
   </si>
   <si>
+    <t>Sum of Amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source </t>
+  </si>
+  <si>
+    <t>Expenditure Type</t>
+  </si>
+  <si>
+    <t>Expenditure sub type</t>
+  </si>
+  <si>
     <t>SOURCE</t>
   </si>
   <si>
@@ -82,7 +96,7 @@
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="43">
+  <fonts count="44">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -262,6 +276,13 @@
       <main:name val="Calibri"/>
       <main:family val="2"/>
       <main:b val="1"/>
+      <main:color theme="1"/>
+      <main:sz val="11"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:name val="Calibri"/>
+      <main:family val="2"/>
       <main:color theme="1"/>
       <main:sz val="11"/>
       <main:scheme val="minor"/>
@@ -366,7 +387,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true"/>
@@ -410,11 +431,12 @@
     <xf numFmtId="0" fontId="37" fillId="3" borderId="0" pivotButton="1" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
     <xf numFmtId="0" fontId="38" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
     <xf numFmtId="0" fontId="39" fillId="3" borderId="0" pivotButton="1" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="40" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="41" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+    <xf numFmtId="0" fontId="40" fillId="3" borderId="0" pivotButton="1" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="41" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="42" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
       <main:alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="42" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="167" fontId="43" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -719,11 +741,165 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" refreshOnLoad="true" refreshedBy="Robert Buczek" refreshedDate="45793.39352048611" createdVersion="7" refreshedVersion="8" minRefreshableVersion="3" recordCount="9387" r:id="4">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:L1048576" sheet="MAIN"/>
+  </cacheSource>
+  <cacheFields count="12">
+    <cacheField name="SOURCE" uniqueList="1" numFmtId="0" sqlType="0" hierarchy="0" level="0" databaseField="1">
+      <sharedItems count="3" containsBlank="1" containsNonDate="0">
+        <m/>
+        <s v="CCMS" u="1"/>
+        <s v="CIS" u="1"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="INV_SOURCE" uniqueList="1" numFmtId="0" sqlType="0" hierarchy="0" level="0" databaseField="1">
+      <sharedItems count="0" containsBlank="1" containsNonDate="0" containsString="0"/>
+    </cacheField>
+    <cacheField name="SUB_SOURCE" uniqueList="1" numFmtId="0" sqlType="0" hierarchy="0" level="0" databaseField="1">
+      <sharedItems count="3" containsBlank="1" containsNonDate="0">
+        <m/>
+        <s v="Applied Receipts" u="1"/>
+        <s v="Expenditure" u="1"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="PAYMENT_DATE" uniqueList="1" numFmtId="0" sqlType="0" hierarchy="0" level="0" databaseField="1">
+      <sharedItems count="0" containsBlank="1" containsNonDate="0" containsString="0"/>
+    </cacheField>
+    <cacheField name="PAYMENT_MONTH" uniqueList="1" numFmtId="0" sqlType="0" hierarchy="0" level="0" databaseField="1">
+      <sharedItems count="23" containsBlank="1" containsDate="1" containsNonDate="0" containsString="0" minDate="2023-04-30T00:00:00" maxDate="2025-05-01T00:00:00">
+        <m/>
+        <d v="2025-04-30T00:00:00" u="1"/>
+        <d v="2024-04-30T00:00:00" u="1"/>
+        <d v="2024-05-31T00:00:00" u="1"/>
+        <d v="2024-06-30T00:00:00" u="1"/>
+        <d v="2024-07-31T00:00:00" u="1"/>
+        <d v="2024-08-31T00:00:00" u="1"/>
+        <d v="2024-09-30T00:00:00" u="1"/>
+        <d v="2024-10-31T00:00:00" u="1"/>
+        <d v="2024-11-30T00:00:00" u="1"/>
+        <d v="2024-12-31T00:00:00" u="1"/>
+        <d v="2023-11-30T00:00:00" u="1"/>
+        <d v="2023-05-31T00:00:00" u="1"/>
+        <d v="2023-09-30T00:00:00" u="1"/>
+        <d v="2024-03-31T00:00:00" u="1"/>
+        <d v="2023-12-31T00:00:00" u="1"/>
+        <d v="2024-01-31T00:00:00" u="1"/>
+        <d v="2024-02-29T00:00:00" u="1"/>
+        <d v="2023-06-30T00:00:00" u="1"/>
+        <d v="2023-10-31T00:00:00" u="1"/>
+        <d v="2023-04-30T00:00:00" u="1"/>
+        <d v="2023-08-31T00:00:00" u="1"/>
+        <d v="2023-07-31T00:00:00" u="1"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="SETTLEMENT_TYPE" uniqueList="1" numFmtId="0" sqlType="0" hierarchy="0" level="0" databaseField="1">
+      <sharedItems count="7" containsBlank="1" containsNonDate="0">
+        <m/>
+        <s v="Applied Receipts" u="1"/>
+        <s v="Voided Payments" u="1"/>
+        <s v="Regular Payments" u="1"/>
+        <s v="Netting Payments" u="1"/>
+        <s v="Refunds" u="1"/>
+        <s v="Voided Refunds" u="1"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="SCHEME" uniqueList="1" numFmtId="0" sqlType="0" hierarchy="0" level="0" databaseField="1">
+      <sharedItems count="4" containsBlank="1" containsNonDate="0">
+        <m/>
+        <s v="Civil" u="1"/>
+        <s v="Crime" u="1"/>
+        <s v="Cfund" u="1"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="SUB_SCHEME" uniqueList="1" numFmtId="0" sqlType="0" hierarchy="0" level="0" databaseField="1">
+      <sharedItems count="6" containsBlank="1" containsNonDate="0">
+        <m/>
+        <s v="Civil Representation" u="1"/>
+        <s v="Legal Help" u="1"/>
+        <s v="Higher Crime" u="1"/>
+        <s v="Lower Crime" u="1"/>
+        <s v="Central Funds" u="1"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="DETAIL_DESC" uniqueList="1" numFmtId="0" sqlType="0" hierarchy="0" level="0" databaseField="1">
+      <sharedItems count="47" containsBlank="1" containsNonDate="0">
+        <m/>
+        <s v="Damages" u="1"/>
+        <s v="Revocation Interest" u="1"/>
+        <s v="Statutory Charge Interest" u="1"/>
+        <s v="Other" u="1"/>
+        <s v="Costs Interest" u="1"/>
+        <s v="Refunds" u="1"/>
+        <s v="Revocation" u="1"/>
+        <s v="Unapplied" u="1"/>
+        <s v="Contributions" u="1"/>
+        <s v="Provider" u="1"/>
+        <s v="Statutory Charge" u="1"/>
+        <s v="Costs" u="1"/>
+        <s v="Monthly Contract Payments" u="1"/>
+        <s v="Recoupments Of Payments On Account" u="1"/>
+        <s v="Default" u="1"/>
+        <s v="Fees/Profit Costs" u="1"/>
+        <s v="Disbursements" u="1"/>
+        <s v="Recovery Of Defence Costs Order" u="1"/>
+        <s v="Cross Examination" u="1"/>
+        <s v="Payments On Account" u="1"/>
+        <s v="Counsel Fees" u="1"/>
+        <s v="Mediation Costs" u="1"/>
+        <s v="Debt Recovery Costs" u="1"/>
+        <s v="Ap Control (Cis)" u="1"/>
+        <s v="Regulation 119 Costs" u="1"/>
+        <s v="Housing Possession Court Duty Scheme" u="1"/>
+        <s v="Litigator Graduated Fee Scheme" u="1"/>
+        <s v="Solicitors Ccu" u="1"/>
+        <s v="Counsel Ccu" u="1"/>
+        <s v="Advocate Graduated Fee Scheme" u="1"/>
+        <s v="Ap To Ar Debt Movement" u="1"/>
+        <s v="Cla Helpline" u="1"/>
+        <s v="Criminal Defence Direct (Cdd)" u="1"/>
+        <s v="Provider Interest" u="1"/>
+        <s v="Family Graduated Fees" u="1"/>
+        <s v="Virtual Court Fees" u="1"/>
+        <s v="Refunds Interest" u="1"/>
+        <s v="Provider Debt Written-Off" u="1"/>
+        <s v="Pre Certificate Costs" u="1"/>
+        <s v="Payments Suspense Account" u="1"/>
+        <s v="Mod Receipt" u="1"/>
+        <s v="Cis Unidentified Receipts" u="1"/>
+        <s v="Balance Sheet Suspense" u="1"/>
+        <s v="Contributions Interest" u="1"/>
+        <s v="Solicitors Standard Fee" u="1"/>
+        <s v="Inquest Payments" u="1"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="CAT_CODE" uniqueList="1" numFmtId="0" sqlType="0" hierarchy="0" level="0" databaseField="1">
+      <sharedItems count="0" containsBlank="1" containsNonDate="0" containsString="0"/>
+    </cacheField>
+    <cacheField name="AP_AR_MOVEMENT" uniqueList="1" numFmtId="0" sqlType="0" hierarchy="0" level="0" databaseField="1">
+      <sharedItems count="3" containsBlank="1" containsNonDate="0">
+        <m/>
+        <s v="N" u="1"/>
+        <s v="Y" u="1"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="TOTAL" uniqueList="1" numFmtId="0" sqlType="0" hierarchy="0" level="0" databaseField="1">
+      <sharedItems count="0" containsBlank="1" containsNonDate="0" containsString="0"/>
+    </cacheField>
+  </cacheFields>
+</pivotCacheDefinition>
+</file>
+
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -876,7 +1052,142 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Transparency rec pivot" cacheId="3" dataOnRows="0" dataCaption="Values" showError="0" showMissing="1" updatedVersion="8" minRefreshableVersion="3" asteriskTotals="0" showItems="1" editData="0" disableFieldList="0" showCalcMbrs="0" visualTotals="1" showMultipleLabel="1" showDataDropDown="1" showDrill="1" printDrill="0" showMemberPropertyTips="1" showDataTips="1" enableWizard="1" enableDrill="1" enableFieldProperties="1" preserveFormatting="1" useAutoFormatting="1" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" rowGrandTotals="1" colGrandTotals="1" fieldPrintTitles="0" itemPrintTitles="1" mergeItem="0" showDropZones="1" createdVersion="3" indent="0" showEmptyRow="0" showEmptyCol="0" showHeaders="1" compact="1" outline="1" outlineData="1" compactData="1" published="0" gridDropZones="0" immersive="1" multipleFieldFilters="0" chartFormat="0" fieldListSortAscending="0" mdxSubqueries="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" r:id="rId1">
+<pivotTableDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SourceNType" cacheId="3" dataOnRows="0" dataCaption="Values" showError="0" showMissing="1" updatedVersion="8" minRefreshableVersion="3" asteriskTotals="0" showItems="1" editData="0" disableFieldList="0" showCalcMbrs="0" visualTotals="1" showMultipleLabel="1" showDataDropDown="1" showDrill="1" printDrill="0" showMemberPropertyTips="1" showDataTips="1" enableWizard="1" enableDrill="1" enableFieldProperties="1" preserveFormatting="1" useAutoFormatting="1" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" rowGrandTotals="0" colGrandTotals="0" fieldPrintTitles="0" itemPrintTitles="1" mergeItem="0" showDropZones="1" createdVersion="3" indent="0" showEmptyRow="0" showEmptyCol="0" showHeaders="1" compact="0" outline="0" outlineData="0" compactData="0" published="0" gridDropZones="1" immersive="1" multipleFieldFilters="0" chartFormat="0" fieldListSortAscending="0" mdxSubqueries="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" r:id="rId1">
+  <location ref="A5:E7" firstHeaderRow="1" firstDataRow="2" firstDataCol="4"/>
+  <pivotFields count="12">
+    <pivotField name="Source " axis="axisRow" showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="0">
+      <items count="3">
+        <item t="data" h="1" sd="1" m="1" x="1"/>
+        <item t="data" sd="1" m="1" x="2"/>
+        <item t="data" h="1" sd="1" x="0"/>
+      </items>
+    </pivotField>
+    <pivotField showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1"/>
+    <pivotField name="Expenditure Type" axis="axisRow" showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1">
+      <items count="4">
+        <item t="data" sd="1" m="1" x="1"/>
+        <item t="data" sd="1" m="1" x="2"/>
+        <item t="data" sd="1" x="0"/>
+        <item t="default" sd="1"/>
+      </items>
+    </pivotField>
+    <pivotField showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1"/>
+    <pivotField name="Month" axis="axisCol" showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1">
+      <items count="24">
+        <item t="data" sd="1" m="1" x="22"/>
+        <item t="data" sd="1" x="0"/>
+        <item t="data" sd="1" m="1" x="21"/>
+        <item t="data" sd="1" m="1" x="20"/>
+        <item t="data" sd="1" m="1" x="12"/>
+        <item t="data" sd="1" m="1" x="18"/>
+        <item t="data" sd="1" m="1" x="13"/>
+        <item t="data" sd="1" m="1" x="19"/>
+        <item t="data" sd="1" m="1" x="11"/>
+        <item t="data" sd="1" m="1" x="15"/>
+        <item t="data" sd="1" m="1" x="16"/>
+        <item t="data" sd="1" m="1" x="17"/>
+        <item t="data" sd="1" m="1" x="14"/>
+        <item t="data" sd="1" m="1" x="2"/>
+        <item t="data" sd="1" m="1" x="3"/>
+        <item t="data" sd="1" m="1" x="4"/>
+        <item t="data" sd="1" m="1" x="5"/>
+        <item t="data" sd="1" m="1" x="6"/>
+        <item t="data" sd="1" m="1" x="7"/>
+        <item t="data" sd="1" m="1" x="8"/>
+        <item t="data" sd="1" m="1" x="9"/>
+        <item t="data" sd="1" m="1" x="10"/>
+        <item t="data" sd="1" m="1" x="1"/>
+        <item t="default" sd="1"/>
+      </items>
+    </pivotField>
+    <pivotField name="Expenditure sub type" axis="axisRow" showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1">
+      <items count="8">
+        <item t="data" sd="1" m="1" x="1"/>
+        <item t="data" sd="1" m="1" x="4"/>
+        <item t="data" sd="1" m="1" x="5"/>
+        <item t="data" sd="1" m="1" x="3"/>
+        <item t="data" sd="1" m="1" x="2"/>
+        <item t="data" sd="1" m="1" x="6"/>
+        <item t="data" sd="1" x="0"/>
+        <item t="default" sd="1"/>
+      </items>
+    </pivotField>
+    <pivotField showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1"/>
+    <pivotField showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1"/>
+    <pivotField name="Description" axis="axisRow" showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1">
+      <items count="48">
+        <item t="data" sd="1" m="1" x="30"/>
+        <item t="data" sd="1" m="1" x="24"/>
+        <item t="data" sd="1" m="1" x="31"/>
+        <item t="data" sd="1" m="1" x="42"/>
+        <item t="data" sd="1" m="1" x="32"/>
+        <item t="data" sd="1" m="1" x="9"/>
+        <item t="data" sd="1" m="1" x="12"/>
+        <item t="data" sd="1" m="1" x="5"/>
+        <item t="data" sd="1" m="1" x="29"/>
+        <item t="data" sd="1" m="1" x="21"/>
+        <item t="data" sd="1" m="1" x="33"/>
+        <item t="data" sd="1" m="1" x="19"/>
+        <item t="data" sd="1" m="1" x="1"/>
+        <item t="data" sd="1" m="1" x="23"/>
+        <item t="data" sd="1" m="1" x="15"/>
+        <item t="data" sd="1" m="1" x="17"/>
+        <item t="data" sd="1" m="1" x="35"/>
+        <item t="data" sd="1" m="1" x="16"/>
+        <item t="data" sd="1" m="1" x="26"/>
+        <item t="data" sd="1" m="1" x="27"/>
+        <item t="data" sd="1" m="1" x="22"/>
+        <item t="data" sd="1" m="1" x="13"/>
+        <item t="data" sd="1" m="1" x="4"/>
+        <item t="data" sd="1" m="1" x="20"/>
+        <item t="data" sd="1" m="1" x="10"/>
+        <item t="data" sd="1" m="1" x="14"/>
+        <item t="data" sd="1" m="1" x="18"/>
+        <item t="data" sd="1" m="1" x="6"/>
+        <item t="data" sd="1" m="1" x="25"/>
+        <item t="data" sd="1" m="1" x="7"/>
+        <item t="data" sd="1" m="1" x="2"/>
+        <item t="data" sd="1" m="1" x="28"/>
+        <item t="data" sd="1" m="1" x="11"/>
+        <item t="data" sd="1" m="1" x="3"/>
+        <item t="data" sd="1" m="1" x="8"/>
+        <item t="data" sd="1" m="1" x="36"/>
+        <item t="data" sd="1" x="0"/>
+        <item t="data" sd="1" m="1" x="43"/>
+        <item t="data" sd="1" m="1" x="38"/>
+        <item t="data" sd="1" m="1" x="39"/>
+        <item t="data" sd="1" m="1" x="41"/>
+        <item t="data" sd="1" m="1" x="46"/>
+        <item t="data" sd="1" m="1" x="34"/>
+        <item t="data" sd="1" m="1" x="40"/>
+        <item t="data" sd="1" m="1" x="37"/>
+        <item t="data" sd="1" m="1" x="44"/>
+        <item t="data" sd="1" m="1" x="45"/>
+        <item t="default" sd="1"/>
+      </items>
+    </pivotField>
+    <pivotField showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1"/>
+    <pivotField showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1"/>
+    <pivotField dataField="1" showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1"/>
+  </pivotFields>
+  <rowFields count="4">
+    <field x="0"/>
+    <field x="2"/>
+    <field x="5"/>
+    <field x="8"/>
+  </rowFields>
+  <colFields count="1">
+    <field x="4"/>
+  </colFields>
+  <dataFields count="1">
+    <dataField name="Sum of Amount" fld="11" subtotal="sum" showDataAs="normal" baseField="8" baseItem="33" numFmtId="8"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Transparency rec pivot" cacheId="4" dataOnRows="0" dataCaption="Values" showError="0" showMissing="1" updatedVersion="8" minRefreshableVersion="3" asteriskTotals="0" showItems="1" editData="0" disableFieldList="0" showCalcMbrs="0" visualTotals="1" showMultipleLabel="1" showDataDropDown="1" showDrill="1" printDrill="0" showMemberPropertyTips="1" showDataTips="1" enableWizard="1" enableDrill="1" enableFieldProperties="1" preserveFormatting="1" useAutoFormatting="1" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" rowGrandTotals="1" colGrandTotals="1" fieldPrintTitles="0" itemPrintTitles="1" mergeItem="0" showDropZones="1" createdVersion="3" indent="0" showEmptyRow="0" showEmptyCol="0" showHeaders="1" compact="1" outline="1" outlineData="1" compactData="1" published="0" gridDropZones="0" immersive="1" multipleFieldFilters="0" chartFormat="0" fieldListSortAscending="0" mdxSubqueries="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" r:id="rId1">
   <location ref="A5:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="12">
     <pivotField axis="axisPage" showDropDowns="1" compact="1" outline="1" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1">
@@ -2368,6 +2679,65 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="false"/>
   </sheetPr>
+  <dimension ref="A1:L6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" customWidth="true"/>
+    <col min="2" max="2" width="21.1640625" customWidth="true"/>
+    <col min="3" max="3" width="22.5" customWidth="true"/>
+    <col min="4" max="4" width="12.6640625" customWidth="true"/>
+    <col min="5" max="5" width="9.0" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0"/>
+      <c r="B1" s="0"/>
+      <c r="C1" s="0"/>
+      <c r="D1" s="0"/>
+      <c r="E1" s="0"/>
+      <c r="F1" s="0"/>
+      <c r="G1" s="0"/>
+      <c r="H1" s="0"/>
+      <c r="I1" s="0"/>
+      <c r="J1" s="0"/>
+      <c r="K1" s="0"/>
+      <c r="L1" s="0"/>
+    </row>
+    <row r="5" ht="15.0" customHeight="true" hidden="false">
+      <c r="A5" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="42" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" ht="15.0" customHeight="true" hidden="false">
+      <c r="A6" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="42" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr autoPageBreaks="false"/>
+  </sheetPr>
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2393,40 +2763,40 @@
       <c r="L1" s="0"/>
     </row>
     <row r="2" ht="15.0" customHeight="true" hidden="false">
-      <c r="A2" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="43" t="s">
+      <c r="A2" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="44" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" ht="15.0" customHeight="true" hidden="false">
-      <c r="A3" s="42" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="43" t="s">
+      <c r="A3" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="44" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" ht="15.0" customHeight="true" hidden="false">
-      <c r="A5" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="43" t="s">
-        <v>15</v>
+      <c r="A5" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="44" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6" ht="15.0" customHeight="true" hidden="false">
-      <c r="A6" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="45"/>
+      <c r="A6" s="45" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="46"/>
     </row>
     <row r="7" ht="15.0" customHeight="true" hidden="false">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="45"/>
+      <c r="B7" s="46"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>